<commit_message>
fixing full moon dataset
</commit_message>
<xml_diff>
--- a/FullMoons2009.xlsx
+++ b/FullMoons2009.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b954984cd282067a/Desktop/Class_folder/Class Project/Horrorscopes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46752C91-3E91-433A-95FF-39336BFECB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{46752C91-3E91-433A-95FF-39336BFECB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D541FCB3-F481-4298-9C90-A06F415C4FD4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E9F8E573-3901-46DA-AE72-050C917F508D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Full Moon Dates" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Full Moon Dates'!$A$1:$C$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Full Moon Dates'!$A$1:$C$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713C195E-CCF5-45CC-B378-B2E41D691E6A}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,15 +593,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>40178</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
@@ -636,13 +628,10 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C26" xr:uid="{713C195E-CCF5-45CC-B378-B2E41D691E6A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C26">
-      <sortCondition ref="B1:B26"/>
+  <autoFilter ref="A1:C25" xr:uid="{713C195E-CCF5-45CC-B378-B2E41D691E6A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
+      <sortCondition ref="B1:B25"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>